<commit_message>
move handle.docx to app
</commit_message>
<xml_diff>
--- a/new_file.xlsx
+++ b/new_file.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -809,6 +809,100 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Mặt sau</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>PHAM DUY LONG</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>S Trà Co, Thanh Cái, Qung NInh phó Móng Khu Trang Ginl Trà Co, Thanh Móng Cál, phó</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>03/12/2006</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>022206004066</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0v12/2031</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Việt Nam</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Hải Xuan, Thành phố Móng Cái, Quảng Ninh Hải Xuán, Thành phó Móng Cá</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Mặt sau</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>PHAM DUY LONG</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>S Trà Co, Thanh Cái, Qung NInh phó Móng Khu Trang Ginl Trà Co, Thanh Móng Cál, phó</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>03/12/2006</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>022206004066</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0v12/2031</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Việt Nam</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Hải Xuan, Thành phố Móng Cái, Quảng Ninh Hải Xuán, Thành phó Móng Cá</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add converBase64 and test, cor error
</commit_message>
<xml_diff>
--- a/new_file.xlsx
+++ b/new_file.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -903,6 +903,53 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Mặt sau</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>PHAM DUY LONG</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>S Trà Co, Thanh Cái, Qung NInh phó Móng Khu Trang Ginl Trà Co, Thanh Móng Cál, phó</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>03/12/2006</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>022206004066</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>0v12/2031</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Việt Nam</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Hải Xuan, Thành phố Móng Cái, Quảng Ninh Hải Xuán, Thành phó Móng Cá</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Nam</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>